<commit_message>
Adding UI feedback when registering and editing
</commit_message>
<xml_diff>
--- a/hoja.xlsx
+++ b/hoja.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
   <si>
     <t/>
   </si>
@@ -83,18 +83,6 @@
     <t>ICBF</t>
   </si>
   <si>
-    <t>CAVIEDEZ FERNANDEZ</t>
-  </si>
-  <si>
-    <t>JUAN SEBASTIAN</t>
-  </si>
-  <si>
-    <t>OPERARIO</t>
-  </si>
-  <si>
-    <t>DIRECTA</t>
-  </si>
-  <si>
     <t>CORDOBA ERAZO</t>
   </si>
   <si>
@@ -105,9 +93,6 @@
   </si>
   <si>
     <t>INDIRECTA</t>
-  </si>
-  <si>
-    <t>MANUEL ALEJANDRO</t>
   </si>
 </sst>
 </file>
@@ -170,35 +155,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:W5"/>
+  <dimension ref="A1:W3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="21.16796875" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="20.19140625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="16.66796875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="11.70703125" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="12.125" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="14.58984375" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="12.171875" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="9.390625" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="10.8359375" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="12.171875" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="9.390625" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="9.390625" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" width="11.0546875" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="9.390625" customWidth="true" bestFit="true"/>
-    <col min="12" max="12" width="11.0546875" customWidth="true" bestFit="true"/>
-    <col min="13" max="13" width="11.0546875" customWidth="true" bestFit="true"/>
-    <col min="14" max="14" width="11.0546875" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="11.0546875" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="8.27734375" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="9.109375" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" width="8.27734375" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="7.01171875" customWidth="true" bestFit="true"/>
+    <col min="12" max="12" width="9.390625" customWidth="true" bestFit="true"/>
+    <col min="13" max="13" width="8.27734375" customWidth="true" bestFit="true"/>
+    <col min="14" max="14" width="9.390625" customWidth="true" bestFit="true"/>
     <col min="15" max="15" width="11.30859375" customWidth="true" bestFit="true"/>
     <col min="16" max="16" width="13.16015625" customWidth="true" bestFit="true"/>
     <col min="17" max="17" width="12.6953125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="13.203125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="9.390625" customWidth="true" bestFit="true"/>
     <col min="20" max="20" width="11.10546875" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="9.390625" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="11.0546875" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="6.8359375" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="5.81640625" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="4.97265625" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="8.27734375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -329,194 +314,61 @@
         <v>26</v>
       </c>
       <c r="E3" s="6" t="n">
-        <v>1203111.0</v>
+        <v>996666.6666666666</v>
       </c>
       <c r="F3" s="6" t="n">
-        <v>103111.0</v>
+        <v>107797.0</v>
       </c>
       <c r="G3" s="6" t="n">
-        <v>1203111.0</v>
+        <v>1104463.6666666665</v>
       </c>
       <c r="H3" t="n" s="6">
-        <v>44000.0</v>
+        <v>39866.666666666664</v>
       </c>
       <c r="I3" t="n" s="6">
-        <v>44000.0</v>
+        <v>39866.666666666664</v>
       </c>
       <c r="J3" t="n" s="6">
-        <v>88000.0</v>
+        <v>79733.33333333333</v>
       </c>
       <c r="K3" s="6" t="n">
         <v>0.0</v>
       </c>
       <c r="L3" s="6" t="n">
-        <v>132000.0</v>
+        <v>119599.99999999999</v>
       </c>
       <c r="M3" s="6" t="n">
-        <v>158796.0</v>
+        <v>10405.199999999999</v>
       </c>
       <c r="N3" s="6" t="n">
-        <v>100219.1463</v>
+        <v>130005.19999999998</v>
       </c>
       <c r="O3" s="6" t="n">
-        <v>100219.1463</v>
+        <v>92001.82343333332</v>
       </c>
       <c r="P3" s="6" t="n">
-        <v>45870.0</v>
+        <v>92001.82343333332</v>
       </c>
       <c r="Q3" s="6" t="n">
-        <v>12031.11</v>
+        <v>41561.0</v>
       </c>
       <c r="R3" s="6" t="n">
-        <v>258339.40259999997</v>
+        <v>11044.636666666665</v>
       </c>
       <c r="S3" s="6" t="n">
-        <v>44000.0</v>
+        <v>236609.2835333333</v>
       </c>
       <c r="T3" s="6" t="n">
-        <v>0.0</v>
+        <v>39866.666666666664</v>
       </c>
       <c r="U3" s="6" t="n">
         <v>0.0</v>
       </c>
       <c r="V3" s="6" t="n">
-        <v>44000.0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s" s="6">
-        <v>27</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" t="s" s="6">
-        <v>30</v>
-      </c>
-      <c r="E4" s="6" t="n">
-        <v>1056444.3333333335</v>
-      </c>
-      <c r="F4" s="6" t="n">
-        <v>103111.0</v>
-      </c>
-      <c r="G4" s="6" t="n">
-        <v>1056444.3333333335</v>
-      </c>
-      <c r="H4" t="n" s="6">
-        <v>38133.333333333336</v>
-      </c>
-      <c r="I4" t="n" s="6">
-        <v>38133.333333333336</v>
-      </c>
-      <c r="J4" t="n" s="6">
-        <v>76266.66666666667</v>
-      </c>
-      <c r="K4" s="6" t="n">
         <v>0.0</v>
       </c>
-      <c r="L4" s="6" t="n">
-        <v>114400.0</v>
-      </c>
-      <c r="M4" s="6" t="n">
-        <v>137623.2</v>
-      </c>
-      <c r="N4" s="6" t="n">
-        <v>88001.81296666668</v>
-      </c>
-      <c r="O4" s="6" t="n">
-        <v>88001.81296666668</v>
-      </c>
-      <c r="P4" s="6" t="n">
-        <v>39754.0</v>
-      </c>
-      <c r="Q4" s="6" t="n">
-        <v>10564.443333333335</v>
-      </c>
-      <c r="R4" s="6" t="n">
-        <v>226322.0692666667</v>
-      </c>
-      <c r="S4" s="6" t="n">
-        <v>38133.333333333336</v>
-      </c>
-      <c r="T4" s="6" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="U4" s="6" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="V4" s="6" t="n">
-        <v>38133.333333333336</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s" s="6">
-        <v>23</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" t="s" s="6">
-        <v>26</v>
-      </c>
-      <c r="E5" s="6" t="n">
-        <v>1.32E7</v>
-      </c>
-      <c r="F5" s="6" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G5" s="6" t="n">
-        <v>1.32E7</v>
-      </c>
-      <c r="H5" t="n" s="6">
-        <v>528000.0</v>
-      </c>
-      <c r="I5" t="n" s="6">
-        <v>528000.0</v>
-      </c>
-      <c r="J5" t="n" s="6">
-        <v>1056000.0</v>
-      </c>
-      <c r="K5" s="6" t="n">
-        <v>528000.0</v>
-      </c>
-      <c r="L5" s="6" t="n">
-        <v>1584000.0</v>
-      </c>
-      <c r="M5" s="6" t="n">
-        <v>2433552.0</v>
-      </c>
-      <c r="N5" s="6" t="n">
-        <v>1099560.0</v>
-      </c>
-      <c r="O5" s="6" t="n">
-        <v>1099560.0</v>
-      </c>
-      <c r="P5" s="6" t="n">
-        <v>550440.0</v>
-      </c>
-      <c r="Q5" s="6" t="n">
-        <v>132000.0</v>
-      </c>
-      <c r="R5" s="6" t="n">
-        <v>2881560.0</v>
-      </c>
-      <c r="S5" s="6" t="n">
-        <v>528000.0</v>
-      </c>
-      <c r="T5" s="6" t="n">
-        <v>264000.0</v>
-      </c>
-      <c r="U5" s="6" t="n">
-        <v>396000.0</v>
-      </c>
-      <c r="V5" s="6" t="n">
-        <v>1188000.0</v>
+      <c r="W3" s="6" t="n">
+        <v>39866.666666666664</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
only name and only lastname allowed
</commit_message>
<xml_diff>
--- a/hoja.xlsx
+++ b/hoja.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
   <si>
     <t/>
   </si>
@@ -93,6 +93,18 @@
   </si>
   <si>
     <t>INDIRECTA</t>
+  </si>
+  <si>
+    <t>CAVIEDEZ FERNANDEZ</t>
+  </si>
+  <si>
+    <t>JUAN SEBASTIAN</t>
+  </si>
+  <si>
+    <t>OPERARIO</t>
+  </si>
+  <si>
+    <t>DIRECTA</t>
   </si>
 </sst>
 </file>
@@ -155,35 +167,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:W3"/>
+  <dimension ref="A1:W4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="16.66796875" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="11.70703125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="21.16796875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="16.2265625" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="12.125" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="14.58984375" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="9.390625" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="12.171875" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="10.8359375" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="11.0546875" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="8.27734375" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="9.109375" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" width="8.27734375" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="7.01171875" customWidth="true" bestFit="true"/>
-    <col min="12" max="12" width="9.390625" customWidth="true" bestFit="true"/>
-    <col min="13" max="13" width="8.27734375" customWidth="true" bestFit="true"/>
-    <col min="14" max="14" width="9.390625" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="12.171875" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="9.390625" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="9.390625" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" width="11.0546875" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="11.0546875" customWidth="true" bestFit="true"/>
+    <col min="12" max="12" width="11.0546875" customWidth="true" bestFit="true"/>
+    <col min="13" max="13" width="9.390625" customWidth="true" bestFit="true"/>
+    <col min="14" max="14" width="11.0546875" customWidth="true" bestFit="true"/>
     <col min="15" max="15" width="11.30859375" customWidth="true" bestFit="true"/>
     <col min="16" max="16" width="13.16015625" customWidth="true" bestFit="true"/>
     <col min="17" max="17" width="12.6953125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="13.203125" customWidth="true" bestFit="true"/>
-    <col min="19" max="19" width="9.390625" customWidth="true" bestFit="true"/>
+    <col min="19" max="19" width="11.0546875" customWidth="true" bestFit="true"/>
     <col min="20" max="20" width="11.10546875" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="5.81640625" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="4.97265625" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="8.27734375" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="9.390625" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="9.390625" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="11.0546875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -338,10 +350,10 @@
         <v>119599.99999999999</v>
       </c>
       <c r="M3" s="6" t="n">
-        <v>10405.199999999999</v>
+        <v>5202.599999999999</v>
       </c>
       <c r="N3" s="6" t="n">
-        <v>130005.19999999998</v>
+        <v>124802.59999999999</v>
       </c>
       <c r="O3" s="6" t="n">
         <v>92001.82343333332</v>
@@ -369,6 +381,77 @@
       </c>
       <c r="W3" s="6" t="n">
         <v>39866.666666666664</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" t="s" s="6">
+        <v>30</v>
+      </c>
+      <c r="E4" s="6" t="n">
+        <v>1.5333333333333334E7</v>
+      </c>
+      <c r="F4" s="6" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G4" s="6" t="n">
+        <v>1.5333333333333334E7</v>
+      </c>
+      <c r="H4" t="n" s="6">
+        <v>613333.3333333334</v>
+      </c>
+      <c r="I4" t="n" s="6">
+        <v>613333.3333333334</v>
+      </c>
+      <c r="J4" t="n" s="6">
+        <v>1226666.6666666667</v>
+      </c>
+      <c r="K4" s="6" t="n">
+        <v>1303333.3333333335</v>
+      </c>
+      <c r="L4" s="6" t="n">
+        <v>1840000.0</v>
+      </c>
+      <c r="M4" s="6" t="n">
+        <v>373520.0</v>
+      </c>
+      <c r="N4" s="6" t="n">
+        <v>3516853.3333333335</v>
+      </c>
+      <c r="O4" s="6" t="n">
+        <v>1277266.6666666667</v>
+      </c>
+      <c r="P4" s="6" t="n">
+        <v>1277266.6666666667</v>
+      </c>
+      <c r="Q4" s="6" t="n">
+        <v>639400.0</v>
+      </c>
+      <c r="R4" s="6" t="n">
+        <v>153333.33333333334</v>
+      </c>
+      <c r="S4" s="6" t="n">
+        <v>3347266.666666667</v>
+      </c>
+      <c r="T4" s="6" t="n">
+        <v>613333.3333333334</v>
+      </c>
+      <c r="U4" s="6" t="n">
+        <v>306666.6666666667</v>
+      </c>
+      <c r="V4" s="6" t="n">
+        <v>460000.0</v>
+      </c>
+      <c r="W4" s="6" t="n">
+        <v>1380000.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>